<commit_message>
Update & resolving merge conflicts
</commit_message>
<xml_diff>
--- a/reporting/project_schedule/project_schedule_v1.xlsx
+++ b/reporting/project_schedule/project_schedule_v1.xlsx
@@ -1361,6 +1361,141 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="11">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="19" xfId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="11" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="23" xfId="12">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="19" xfId="13" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="14" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="20" xfId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="21" xfId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="22" xfId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="20" xfId="13" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1378,141 +1513,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="22" xfId="12" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="20" xfId="12" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="21" xfId="12" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="22" xfId="12" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="23" xfId="12">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="19" xfId="13" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="14" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="11" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="19" xfId="12" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1657,7 +1657,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="Ausgewählter_Zeitraum" max="100" min="1" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="Ausgewählter_Zeitraum" max="100" min="1" page="10" val="6"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1945,7 +1945,7 @@
   <dimension ref="A1:EX58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+      <selection activeCell="AA41" sqref="AA41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1972,18 +1972,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:93" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
       <c r="E1" s="39"/>
       <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:93" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
       <c r="E2" s="37" t="s">
         <v>96</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
       <c r="F4" s="36">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -2248,11 +2248,11 @@
       <c r="B7" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="128">
+      <c r="D7" s="144">
         <v>42660</v>
       </c>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2328,11 +2328,11 @@
       <c r="B8" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="129">
+      <c r="D8" s="145">
         <v>42842</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="130"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2667,11 +2667,11 @@
         <v>1</v>
       </c>
       <c r="C12" s="35"/>
-      <c r="D12" s="131" t="s">
+      <c r="D12" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
       <c r="G12" s="44"/>
       <c r="H12" s="35" t="s">
         <v>23</v>
@@ -2688,14 +2688,14 @@
       <c r="R12" s="65"/>
       <c r="S12" s="65"/>
       <c r="T12" s="65"/>
-      <c r="U12" s="131" t="s">
+      <c r="U12" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="V12" s="131"/>
-      <c r="W12" s="131"/>
-      <c r="X12" s="131"/>
-      <c r="Y12" s="131"/>
-      <c r="Z12" s="131"/>
+      <c r="V12" s="115"/>
+      <c r="W12" s="115"/>
+      <c r="X12" s="115"/>
+      <c r="Y12" s="115"/>
+      <c r="Z12" s="115"/>
       <c r="AA12" s="58"/>
       <c r="AB12" s="35" t="s">
         <v>28</v>
@@ -2712,12 +2712,12 @@
       <c r="AL12" s="65"/>
       <c r="AM12" s="65"/>
       <c r="AN12" s="65"/>
-      <c r="AO12" s="131"/>
-      <c r="AP12" s="131"/>
-      <c r="AQ12" s="131"/>
-      <c r="AR12" s="131"/>
-      <c r="AS12" s="131"/>
-      <c r="AT12" s="131"/>
+      <c r="AO12" s="115"/>
+      <c r="AP12" s="115"/>
+      <c r="AQ12" s="115"/>
+      <c r="AR12" s="115"/>
+      <c r="AS12" s="115"/>
+      <c r="AT12" s="115"/>
       <c r="AU12" s="44"/>
       <c r="AV12" s="35"/>
       <c r="AW12" s="35"/>
@@ -2732,12 +2732,12 @@
       <c r="BF12" s="65"/>
       <c r="BG12" s="65"/>
       <c r="BH12" s="65"/>
-      <c r="BI12" s="131"/>
-      <c r="BJ12" s="131"/>
-      <c r="BK12" s="131"/>
-      <c r="BL12" s="131"/>
-      <c r="BM12" s="131"/>
-      <c r="BN12" s="131"/>
+      <c r="BI12" s="115"/>
+      <c r="BJ12" s="115"/>
+      <c r="BK12" s="115"/>
+      <c r="BL12" s="115"/>
+      <c r="BM12" s="115"/>
+      <c r="BN12" s="115"/>
       <c r="BO12" s="14"/>
       <c r="BP12" s="14"/>
       <c r="BQ12" s="14"/>
@@ -2772,57 +2772,57 @@
         <v>16</v>
       </c>
       <c r="C13" s="49"/>
-      <c r="D13" s="146" t="s">
+      <c r="D13" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="146"/>
-      <c r="F13" s="146"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
       <c r="G13" s="44"/>
-      <c r="H13" s="133" t="s">
+      <c r="H13" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="133"/>
-      <c r="J13" s="133"/>
-      <c r="K13" s="133"/>
-      <c r="L13" s="133"/>
-      <c r="M13" s="133"/>
-      <c r="N13" s="133"/>
-      <c r="O13" s="133"/>
-      <c r="P13" s="133"/>
-      <c r="Q13" s="133"/>
-      <c r="R13" s="133"/>
-      <c r="S13" s="133"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="114"/>
+      <c r="M13" s="114"/>
+      <c r="N13" s="114"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="114"/>
+      <c r="Q13" s="114"/>
+      <c r="R13" s="114"/>
+      <c r="S13" s="114"/>
       <c r="T13" s="57"/>
-      <c r="U13" s="126" t="s">
+      <c r="U13" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="V13" s="126"/>
-      <c r="W13" s="126"/>
-      <c r="X13" s="126"/>
-      <c r="Y13" s="126"/>
-      <c r="Z13" s="126"/>
+      <c r="V13" s="122"/>
+      <c r="W13" s="122"/>
+      <c r="X13" s="122"/>
+      <c r="Y13" s="122"/>
+      <c r="Z13" s="122"/>
       <c r="AA13" s="58"/>
-      <c r="AB13" s="149" t="s">
+      <c r="AB13" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="AC13" s="149"/>
-      <c r="AD13" s="149"/>
-      <c r="AE13" s="149"/>
-      <c r="AF13" s="149"/>
-      <c r="AG13" s="149"/>
-      <c r="AH13" s="149"/>
-      <c r="AI13" s="149"/>
-      <c r="AJ13" s="149"/>
-      <c r="AK13" s="149"/>
-      <c r="AL13" s="149"/>
-      <c r="AM13" s="149"/>
+      <c r="AC13" s="128"/>
+      <c r="AD13" s="128"/>
+      <c r="AE13" s="128"/>
+      <c r="AF13" s="128"/>
+      <c r="AG13" s="128"/>
+      <c r="AH13" s="128"/>
+      <c r="AI13" s="128"/>
+      <c r="AJ13" s="128"/>
+      <c r="AK13" s="128"/>
+      <c r="AL13" s="128"/>
+      <c r="AM13" s="128"/>
       <c r="AN13" s="44"/>
       <c r="AO13" s="44"/>
       <c r="AP13" s="44"/>
-      <c r="AQ13" s="151">
+      <c r="AQ13" s="130">
         <v>900</v>
       </c>
-      <c r="AR13" s="151"/>
+      <c r="AR13" s="130"/>
       <c r="AS13" s="57" t="s">
         <v>14</v>
       </c>
@@ -2838,21 +2838,21 @@
       <c r="BA13" s="44"/>
       <c r="BB13" s="44"/>
       <c r="BC13" s="44"/>
-      <c r="BD13" s="134" t="s">
+      <c r="BD13" s="148" t="s">
         <v>76</v>
       </c>
-      <c r="BE13" s="134"/>
-      <c r="BF13" s="134"/>
-      <c r="BG13" s="134"/>
-      <c r="BH13" s="136">
+      <c r="BE13" s="148"/>
+      <c r="BF13" s="148"/>
+      <c r="BG13" s="148"/>
+      <c r="BH13" s="151">
         <v>42671</v>
       </c>
-      <c r="BI13" s="132"/>
-      <c r="BJ13" s="132"/>
-      <c r="BK13" s="132"/>
-      <c r="BL13" s="132"/>
-      <c r="BM13" s="132"/>
-      <c r="BN13" s="132"/>
+      <c r="BI13" s="147"/>
+      <c r="BJ13" s="147"/>
+      <c r="BK13" s="147"/>
+      <c r="BL13" s="147"/>
+      <c r="BM13" s="147"/>
+      <c r="BN13" s="147"/>
       <c r="BO13" s="14"/>
       <c r="BP13" s="14"/>
       <c r="BQ13" s="14"/>
@@ -2887,57 +2887,57 @@
         <v>17</v>
       </c>
       <c r="C14" s="49"/>
-      <c r="D14" s="147" t="s">
+      <c r="D14" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="147"/>
-      <c r="F14" s="147"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
       <c r="G14" s="44"/>
-      <c r="H14" s="133" t="s">
+      <c r="H14" s="114" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="133"/>
-      <c r="O14" s="133"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="133"/>
-      <c r="S14" s="133"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="114"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="114"/>
+      <c r="M14" s="114"/>
+      <c r="N14" s="114"/>
+      <c r="O14" s="114"/>
+      <c r="P14" s="114"/>
+      <c r="Q14" s="114"/>
+      <c r="R14" s="114"/>
+      <c r="S14" s="114"/>
       <c r="T14" s="57"/>
-      <c r="U14" s="126" t="s">
+      <c r="U14" s="122" t="s">
         <v>94</v>
       </c>
-      <c r="V14" s="126"/>
-      <c r="W14" s="126"/>
-      <c r="X14" s="126"/>
-      <c r="Y14" s="126"/>
-      <c r="Z14" s="126"/>
+      <c r="V14" s="122"/>
+      <c r="W14" s="122"/>
+      <c r="X14" s="122"/>
+      <c r="Y14" s="122"/>
+      <c r="Z14" s="122"/>
       <c r="AA14" s="58"/>
-      <c r="AB14" s="133" t="s">
+      <c r="AB14" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="AC14" s="133"/>
-      <c r="AD14" s="133"/>
-      <c r="AE14" s="133"/>
-      <c r="AF14" s="133"/>
-      <c r="AG14" s="133"/>
-      <c r="AH14" s="133"/>
-      <c r="AI14" s="133"/>
-      <c r="AJ14" s="133"/>
-      <c r="AK14" s="133"/>
-      <c r="AL14" s="133"/>
-      <c r="AM14" s="133"/>
+      <c r="AC14" s="114"/>
+      <c r="AD14" s="114"/>
+      <c r="AE14" s="114"/>
+      <c r="AF14" s="114"/>
+      <c r="AG14" s="114"/>
+      <c r="AH14" s="114"/>
+      <c r="AI14" s="114"/>
+      <c r="AJ14" s="114"/>
+      <c r="AK14" s="114"/>
+      <c r="AL14" s="114"/>
+      <c r="AM14" s="114"/>
       <c r="AN14" s="44"/>
       <c r="AO14" s="44"/>
       <c r="AP14" s="44"/>
-      <c r="AQ14" s="150">
+      <c r="AQ14" s="129">
         <v>42</v>
       </c>
-      <c r="AR14" s="150"/>
+      <c r="AR14" s="129"/>
       <c r="AS14" s="57" t="s">
         <v>14</v>
       </c>
@@ -2953,21 +2953,21 @@
       <c r="BA14" s="63"/>
       <c r="BB14" s="63"/>
       <c r="BC14" s="63"/>
-      <c r="BD14" s="134" t="s">
+      <c r="BD14" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="BE14" s="134"/>
-      <c r="BF14" s="134"/>
-      <c r="BG14" s="134"/>
-      <c r="BH14" s="132" t="s">
+      <c r="BE14" s="148"/>
+      <c r="BF14" s="148"/>
+      <c r="BG14" s="148"/>
+      <c r="BH14" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="BI14" s="132"/>
-      <c r="BJ14" s="132"/>
-      <c r="BK14" s="132"/>
-      <c r="BL14" s="132"/>
-      <c r="BM14" s="132"/>
-      <c r="BN14" s="132"/>
+      <c r="BI14" s="147"/>
+      <c r="BJ14" s="147"/>
+      <c r="BK14" s="147"/>
+      <c r="BL14" s="147"/>
+      <c r="BM14" s="147"/>
+      <c r="BN14" s="147"/>
       <c r="BO14" s="14"/>
       <c r="BP14" s="14"/>
       <c r="BQ14" s="14"/>
@@ -3004,52 +3004,52 @@
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
       <c r="G15" s="44"/>
-      <c r="H15" s="133" t="s">
+      <c r="H15" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
-      <c r="K15" s="133"/>
-      <c r="L15" s="133"/>
-      <c r="M15" s="133"/>
-      <c r="N15" s="133"/>
-      <c r="O15" s="133"/>
-      <c r="P15" s="133"/>
-      <c r="Q15" s="133"/>
-      <c r="R15" s="133"/>
-      <c r="S15" s="133"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="114"/>
+      <c r="O15" s="114"/>
+      <c r="P15" s="114"/>
+      <c r="Q15" s="114"/>
+      <c r="R15" s="114"/>
+      <c r="S15" s="114"/>
       <c r="T15" s="57"/>
-      <c r="U15" s="126" t="s">
+      <c r="U15" s="122" t="s">
         <v>93</v>
       </c>
-      <c r="V15" s="126"/>
-      <c r="W15" s="126"/>
-      <c r="X15" s="126"/>
-      <c r="Y15" s="126"/>
-      <c r="Z15" s="126"/>
+      <c r="V15" s="122"/>
+      <c r="W15" s="122"/>
+      <c r="X15" s="122"/>
+      <c r="Y15" s="122"/>
+      <c r="Z15" s="122"/>
       <c r="AA15" s="58"/>
-      <c r="AB15" s="133" t="s">
+      <c r="AB15" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="AC15" s="133"/>
-      <c r="AD15" s="133"/>
-      <c r="AE15" s="133"/>
-      <c r="AF15" s="133"/>
-      <c r="AG15" s="133"/>
-      <c r="AH15" s="133"/>
-      <c r="AI15" s="133"/>
-      <c r="AJ15" s="133"/>
-      <c r="AK15" s="133"/>
-      <c r="AL15" s="133"/>
-      <c r="AM15" s="133"/>
+      <c r="AC15" s="114"/>
+      <c r="AD15" s="114"/>
+      <c r="AE15" s="114"/>
+      <c r="AF15" s="114"/>
+      <c r="AG15" s="114"/>
+      <c r="AH15" s="114"/>
+      <c r="AI15" s="114"/>
+      <c r="AJ15" s="114"/>
+      <c r="AK15" s="114"/>
+      <c r="AL15" s="114"/>
+      <c r="AM15" s="114"/>
       <c r="AN15" s="44"/>
       <c r="AO15" s="44"/>
       <c r="AP15" s="44"/>
-      <c r="AQ15" s="148">
+      <c r="AQ15" s="127">
         <f>AQ13/AQ14</f>
         <v>21.428571428571427</v>
       </c>
-      <c r="AR15" s="148"/>
+      <c r="AR15" s="127"/>
       <c r="AS15" s="57" t="s">
         <v>29</v>
       </c>
@@ -3065,21 +3065,21 @@
       <c r="BA15" s="63"/>
       <c r="BB15" s="63"/>
       <c r="BC15" s="63"/>
-      <c r="BD15" s="134" t="s">
+      <c r="BD15" s="148" t="s">
         <v>73</v>
       </c>
-      <c r="BE15" s="134"/>
-      <c r="BF15" s="134"/>
-      <c r="BG15" s="134"/>
-      <c r="BH15" s="135" t="s">
+      <c r="BE15" s="148"/>
+      <c r="BF15" s="148"/>
+      <c r="BG15" s="148"/>
+      <c r="BH15" s="149" t="s">
         <v>70</v>
       </c>
-      <c r="BI15" s="135"/>
-      <c r="BJ15" s="135"/>
-      <c r="BK15" s="135"/>
-      <c r="BL15" s="135"/>
-      <c r="BM15" s="135"/>
-      <c r="BN15" s="135"/>
+      <c r="BI15" s="149"/>
+      <c r="BJ15" s="149"/>
+      <c r="BK15" s="149"/>
+      <c r="BL15" s="149"/>
+      <c r="BM15" s="149"/>
+      <c r="BN15" s="149"/>
       <c r="BO15" s="14"/>
       <c r="BP15" s="14"/>
       <c r="BQ15" s="14"/>
@@ -3116,42 +3116,42 @@
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="44"/>
-      <c r="H16" s="133" t="s">
+      <c r="H16" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
-      <c r="K16" s="133"/>
-      <c r="L16" s="133"/>
-      <c r="M16" s="133"/>
-      <c r="N16" s="133"/>
-      <c r="O16" s="133"/>
-      <c r="P16" s="133"/>
-      <c r="Q16" s="133"/>
-      <c r="R16" s="133"/>
-      <c r="S16" s="133"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
+      <c r="N16" s="114"/>
+      <c r="O16" s="114"/>
+      <c r="P16" s="114"/>
+      <c r="Q16" s="114"/>
+      <c r="R16" s="114"/>
+      <c r="S16" s="114"/>
       <c r="T16" s="57"/>
-      <c r="U16" s="127">
+      <c r="U16" s="123">
         <v>42842</v>
       </c>
-      <c r="V16" s="126"/>
-      <c r="W16" s="126"/>
-      <c r="X16" s="126"/>
-      <c r="Y16" s="126"/>
-      <c r="Z16" s="126"/>
+      <c r="V16" s="122"/>
+      <c r="W16" s="122"/>
+      <c r="X16" s="122"/>
+      <c r="Y16" s="122"/>
+      <c r="Z16" s="122"/>
       <c r="AA16" s="58"/>
-      <c r="AB16" s="133"/>
-      <c r="AC16" s="133"/>
-      <c r="AD16" s="133"/>
-      <c r="AE16" s="133"/>
-      <c r="AF16" s="133"/>
-      <c r="AG16" s="133"/>
-      <c r="AH16" s="133"/>
-      <c r="AI16" s="133"/>
-      <c r="AJ16" s="133"/>
-      <c r="AK16" s="133"/>
-      <c r="AL16" s="133"/>
-      <c r="AM16" s="133"/>
+      <c r="AB16" s="114"/>
+      <c r="AC16" s="114"/>
+      <c r="AD16" s="114"/>
+      <c r="AE16" s="114"/>
+      <c r="AF16" s="114"/>
+      <c r="AG16" s="114"/>
+      <c r="AH16" s="114"/>
+      <c r="AI16" s="114"/>
+      <c r="AJ16" s="114"/>
+      <c r="AK16" s="114"/>
+      <c r="AL16" s="114"/>
+      <c r="AM16" s="114"/>
       <c r="AN16" s="57"/>
       <c r="AO16" s="57"/>
       <c r="AP16" s="57"/>
@@ -3168,17 +3168,17 @@
       <c r="BA16" s="60"/>
       <c r="BB16" s="60"/>
       <c r="BC16" s="60"/>
-      <c r="BD16" s="134"/>
-      <c r="BE16" s="134"/>
-      <c r="BF16" s="134"/>
-      <c r="BG16" s="134"/>
-      <c r="BH16" s="116"/>
-      <c r="BI16" s="116"/>
-      <c r="BJ16" s="116"/>
-      <c r="BK16" s="116"/>
-      <c r="BL16" s="116"/>
-      <c r="BM16" s="116"/>
-      <c r="BN16" s="116"/>
+      <c r="BD16" s="148"/>
+      <c r="BE16" s="148"/>
+      <c r="BF16" s="148"/>
+      <c r="BG16" s="148"/>
+      <c r="BH16" s="150"/>
+      <c r="BI16" s="150"/>
+      <c r="BJ16" s="150"/>
+      <c r="BK16" s="150"/>
+      <c r="BL16" s="150"/>
+      <c r="BM16" s="150"/>
+      <c r="BN16" s="150"/>
       <c r="BO16" s="14"/>
       <c r="BP16" s="14"/>
       <c r="BQ16" s="14"/>
@@ -3215,49 +3215,49 @@
       <c r="E17" s="33"/>
       <c r="F17" s="33"/>
       <c r="G17" s="44"/>
-      <c r="H17" s="133" t="s">
+      <c r="H17" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="133"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="133"/>
-      <c r="N17" s="133"/>
-      <c r="O17" s="133"/>
-      <c r="P17" s="133"/>
-      <c r="Q17" s="133"/>
-      <c r="R17" s="133"/>
-      <c r="S17" s="133"/>
+      <c r="I17" s="114"/>
+      <c r="J17" s="114"/>
+      <c r="K17" s="114"/>
+      <c r="L17" s="114"/>
+      <c r="M17" s="114"/>
+      <c r="N17" s="114"/>
+      <c r="O17" s="114"/>
+      <c r="P17" s="114"/>
+      <c r="Q17" s="114"/>
+      <c r="R17" s="114"/>
+      <c r="S17" s="114"/>
       <c r="T17" s="57"/>
-      <c r="U17" s="127">
+      <c r="U17" s="123">
         <v>42871</v>
       </c>
-      <c r="V17" s="126"/>
-      <c r="W17" s="126"/>
-      <c r="X17" s="126"/>
-      <c r="Y17" s="126"/>
-      <c r="Z17" s="126"/>
+      <c r="V17" s="122"/>
+      <c r="W17" s="122"/>
+      <c r="X17" s="122"/>
+      <c r="Y17" s="122"/>
+      <c r="Z17" s="122"/>
       <c r="AA17" s="58"/>
-      <c r="AB17" s="133"/>
-      <c r="AC17" s="133"/>
-      <c r="AD17" s="133"/>
-      <c r="AE17" s="133"/>
-      <c r="AF17" s="133"/>
-      <c r="AG17" s="133"/>
-      <c r="AH17" s="133"/>
-      <c r="AI17" s="133"/>
-      <c r="AJ17" s="133"/>
-      <c r="AK17" s="133"/>
-      <c r="AL17" s="133"/>
-      <c r="AM17" s="133"/>
+      <c r="AB17" s="114"/>
+      <c r="AC17" s="114"/>
+      <c r="AD17" s="114"/>
+      <c r="AE17" s="114"/>
+      <c r="AF17" s="114"/>
+      <c r="AG17" s="114"/>
+      <c r="AH17" s="114"/>
+      <c r="AI17" s="114"/>
+      <c r="AJ17" s="114"/>
+      <c r="AK17" s="114"/>
+      <c r="AL17" s="114"/>
+      <c r="AM17" s="114"/>
       <c r="AN17" s="57"/>
-      <c r="AO17" s="126"/>
-      <c r="AP17" s="126"/>
-      <c r="AQ17" s="126"/>
-      <c r="AR17" s="126"/>
-      <c r="AS17" s="126"/>
-      <c r="AT17" s="126"/>
+      <c r="AO17" s="122"/>
+      <c r="AP17" s="122"/>
+      <c r="AQ17" s="122"/>
+      <c r="AR17" s="122"/>
+      <c r="AS17" s="122"/>
+      <c r="AT17" s="122"/>
       <c r="AU17" s="44"/>
       <c r="AV17" s="60"/>
       <c r="AW17" s="60"/>
@@ -3271,13 +3271,13 @@
       <c r="BE17" s="60"/>
       <c r="BF17" s="60"/>
       <c r="BG17" s="60"/>
-      <c r="BH17" s="116"/>
-      <c r="BI17" s="116"/>
-      <c r="BJ17" s="116"/>
-      <c r="BK17" s="116"/>
-      <c r="BL17" s="116"/>
-      <c r="BM17" s="116"/>
-      <c r="BN17" s="116"/>
+      <c r="BH17" s="150"/>
+      <c r="BI17" s="150"/>
+      <c r="BJ17" s="150"/>
+      <c r="BK17" s="150"/>
+      <c r="BL17" s="150"/>
+      <c r="BM17" s="150"/>
+      <c r="BN17" s="150"/>
       <c r="BO17" s="14"/>
       <c r="BP17" s="14"/>
       <c r="BQ17" s="14"/>
@@ -3317,33 +3317,33 @@
         <v>1</v>
       </c>
       <c r="C21" s="50"/>
-      <c r="D21" s="131" t="s">
+      <c r="D21" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="131"/>
-      <c r="F21" s="131"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
     </row>
     <row r="22" spans="1:154" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="51"/>
-      <c r="D22" s="146" t="s">
+      <c r="D22" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
     </row>
     <row r="23" spans="1:154" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="51" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="51"/>
-      <c r="D23" s="147" t="s">
+      <c r="D23" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="147"/>
-      <c r="F23" s="147"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
     </row>
     <row r="24" spans="1:154" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="31"/>
@@ -3372,75 +3372,75 @@
         <v>19</v>
       </c>
       <c r="F25" s="75"/>
-      <c r="G25" s="145" t="s">
+      <c r="G25" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="145"/>
-      <c r="I25" s="145"/>
-      <c r="J25" s="145"/>
-      <c r="K25" s="145"/>
-      <c r="L25" s="145"/>
-      <c r="M25" s="145"/>
-      <c r="N25" s="145"/>
-      <c r="O25" s="145"/>
-      <c r="P25" s="145" t="s">
+      <c r="H25" s="121"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="121"/>
+      <c r="K25" s="121"/>
+      <c r="L25" s="121"/>
+      <c r="M25" s="121"/>
+      <c r="N25" s="121"/>
+      <c r="O25" s="121"/>
+      <c r="P25" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" s="145"/>
-      <c r="R25" s="145"/>
-      <c r="S25" s="145"/>
-      <c r="T25" s="145"/>
-      <c r="U25" s="145"/>
-      <c r="V25" s="145"/>
-      <c r="W25" s="145"/>
-      <c r="X25" s="145"/>
-      <c r="Y25" s="145"/>
-      <c r="Z25" s="145"/>
-      <c r="AA25" s="145"/>
-      <c r="AB25" s="145"/>
-      <c r="AC25" s="145"/>
-      <c r="AD25" s="145"/>
-      <c r="AE25" s="145"/>
-      <c r="AF25" s="145"/>
-      <c r="AG25" s="140" t="s">
+      <c r="Q25" s="121"/>
+      <c r="R25" s="121"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="121"/>
+      <c r="U25" s="121"/>
+      <c r="V25" s="121"/>
+      <c r="W25" s="121"/>
+      <c r="X25" s="121"/>
+      <c r="Y25" s="121"/>
+      <c r="Z25" s="121"/>
+      <c r="AA25" s="121"/>
+      <c r="AB25" s="121"/>
+      <c r="AC25" s="121"/>
+      <c r="AD25" s="121"/>
+      <c r="AE25" s="121"/>
+      <c r="AF25" s="121"/>
+      <c r="AG25" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="AH25" s="140"/>
-      <c r="AI25" s="140"/>
-      <c r="AJ25" s="140"/>
-      <c r="AK25" s="140"/>
-      <c r="AL25" s="140"/>
-      <c r="AM25" s="140"/>
-      <c r="AN25" s="140"/>
-      <c r="AO25" s="140"/>
-      <c r="AP25" s="140"/>
-      <c r="AQ25" s="140"/>
-      <c r="AR25" s="140"/>
-      <c r="AS25" s="140"/>
-      <c r="AT25" s="140"/>
-      <c r="AU25" s="140"/>
-      <c r="AV25" s="140"/>
-      <c r="AW25" s="140"/>
-      <c r="AX25" s="140" t="s">
+      <c r="AH25" s="137"/>
+      <c r="AI25" s="137"/>
+      <c r="AJ25" s="137"/>
+      <c r="AK25" s="137"/>
+      <c r="AL25" s="137"/>
+      <c r="AM25" s="137"/>
+      <c r="AN25" s="137"/>
+      <c r="AO25" s="137"/>
+      <c r="AP25" s="137"/>
+      <c r="AQ25" s="137"/>
+      <c r="AR25" s="137"/>
+      <c r="AS25" s="137"/>
+      <c r="AT25" s="137"/>
+      <c r="AU25" s="137"/>
+      <c r="AV25" s="137"/>
+      <c r="AW25" s="137"/>
+      <c r="AX25" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="AY25" s="140"/>
-      <c r="AZ25" s="140"/>
-      <c r="BA25" s="140"/>
-      <c r="BB25" s="140"/>
-      <c r="BC25" s="140"/>
-      <c r="BD25" s="140"/>
-      <c r="BE25" s="140"/>
-      <c r="BF25" s="140"/>
-      <c r="BG25" s="140"/>
-      <c r="BH25" s="140"/>
-      <c r="BI25" s="140"/>
-      <c r="BJ25" s="140"/>
-      <c r="BK25" s="140"/>
-      <c r="BL25" s="140"/>
-      <c r="BM25" s="140"/>
-      <c r="BN25" s="140"/>
-      <c r="BO25" s="140"/>
+      <c r="AY25" s="137"/>
+      <c r="AZ25" s="137"/>
+      <c r="BA25" s="137"/>
+      <c r="BB25" s="137"/>
+      <c r="BC25" s="137"/>
+      <c r="BD25" s="137"/>
+      <c r="BE25" s="137"/>
+      <c r="BF25" s="137"/>
+      <c r="BG25" s="137"/>
+      <c r="BH25" s="137"/>
+      <c r="BI25" s="137"/>
+      <c r="BJ25" s="137"/>
+      <c r="BK25" s="137"/>
+      <c r="BL25" s="137"/>
+      <c r="BM25" s="137"/>
+      <c r="BN25" s="137"/>
+      <c r="BO25" s="137"/>
       <c r="BQ25" s="76"/>
       <c r="BR25" s="77"/>
       <c r="BS25" s="14"/>
@@ -3448,81 +3448,81 @@
       <c r="BU25" s="14"/>
       <c r="BV25" s="14"/>
       <c r="BW25" s="14"/>
-      <c r="CJ25" s="117" t="s">
+      <c r="CJ25" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="CK25" s="118"/>
-      <c r="CL25" s="118"/>
-      <c r="CM25" s="118"/>
-      <c r="CN25" s="118"/>
-      <c r="CO25" s="118"/>
-      <c r="CP25" s="118"/>
-      <c r="CQ25" s="118"/>
-      <c r="CR25" s="118"/>
-      <c r="CS25" s="118"/>
-      <c r="CT25" s="118"/>
-      <c r="CU25" s="118"/>
-      <c r="CV25" s="118"/>
-      <c r="CW25" s="118"/>
-      <c r="CX25" s="118"/>
-      <c r="CY25" s="119"/>
-      <c r="CZ25" s="117" t="s">
+      <c r="CK25" s="139"/>
+      <c r="CL25" s="139"/>
+      <c r="CM25" s="139"/>
+      <c r="CN25" s="139"/>
+      <c r="CO25" s="139"/>
+      <c r="CP25" s="139"/>
+      <c r="CQ25" s="139"/>
+      <c r="CR25" s="139"/>
+      <c r="CS25" s="139"/>
+      <c r="CT25" s="139"/>
+      <c r="CU25" s="139"/>
+      <c r="CV25" s="139"/>
+      <c r="CW25" s="139"/>
+      <c r="CX25" s="139"/>
+      <c r="CY25" s="140"/>
+      <c r="CZ25" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="DA25" s="118"/>
-      <c r="DB25" s="118"/>
-      <c r="DC25" s="118"/>
-      <c r="DD25" s="118"/>
-      <c r="DE25" s="118"/>
-      <c r="DF25" s="118"/>
-      <c r="DG25" s="118"/>
-      <c r="DH25" s="118"/>
-      <c r="DI25" s="118"/>
-      <c r="DJ25" s="118"/>
-      <c r="DK25" s="118"/>
-      <c r="DL25" s="118"/>
-      <c r="DM25" s="118"/>
-      <c r="DN25" s="118"/>
-      <c r="DO25" s="118"/>
-      <c r="DP25" s="118"/>
-      <c r="DQ25" s="118"/>
-      <c r="DR25" s="119"/>
-      <c r="DS25" s="117" t="s">
+      <c r="DA25" s="139"/>
+      <c r="DB25" s="139"/>
+      <c r="DC25" s="139"/>
+      <c r="DD25" s="139"/>
+      <c r="DE25" s="139"/>
+      <c r="DF25" s="139"/>
+      <c r="DG25" s="139"/>
+      <c r="DH25" s="139"/>
+      <c r="DI25" s="139"/>
+      <c r="DJ25" s="139"/>
+      <c r="DK25" s="139"/>
+      <c r="DL25" s="139"/>
+      <c r="DM25" s="139"/>
+      <c r="DN25" s="139"/>
+      <c r="DO25" s="139"/>
+      <c r="DP25" s="139"/>
+      <c r="DQ25" s="139"/>
+      <c r="DR25" s="140"/>
+      <c r="DS25" s="138" t="s">
         <v>59</v>
       </c>
-      <c r="DT25" s="118"/>
-      <c r="DU25" s="118"/>
-      <c r="DV25" s="118"/>
-      <c r="DW25" s="118"/>
-      <c r="DX25" s="118"/>
-      <c r="DY25" s="118"/>
-      <c r="DZ25" s="118"/>
-      <c r="EA25" s="118"/>
-      <c r="EB25" s="118"/>
-      <c r="EC25" s="118"/>
-      <c r="ED25" s="118"/>
-      <c r="EE25" s="118"/>
-      <c r="EF25" s="118"/>
-      <c r="EG25" s="118"/>
-      <c r="EH25" s="119"/>
-      <c r="EI25" s="117" t="s">
+      <c r="DT25" s="139"/>
+      <c r="DU25" s="139"/>
+      <c r="DV25" s="139"/>
+      <c r="DW25" s="139"/>
+      <c r="DX25" s="139"/>
+      <c r="DY25" s="139"/>
+      <c r="DZ25" s="139"/>
+      <c r="EA25" s="139"/>
+      <c r="EB25" s="139"/>
+      <c r="EC25" s="139"/>
+      <c r="ED25" s="139"/>
+      <c r="EE25" s="139"/>
+      <c r="EF25" s="139"/>
+      <c r="EG25" s="139"/>
+      <c r="EH25" s="140"/>
+      <c r="EI25" s="138" t="s">
         <v>63</v>
       </c>
-      <c r="EJ25" s="118"/>
-      <c r="EK25" s="118"/>
-      <c r="EL25" s="118"/>
-      <c r="EM25" s="118"/>
-      <c r="EN25" s="118"/>
-      <c r="EO25" s="118"/>
-      <c r="EP25" s="118"/>
-      <c r="EQ25" s="118"/>
-      <c r="ER25" s="118"/>
-      <c r="ES25" s="118"/>
-      <c r="ET25" s="118"/>
-      <c r="EU25" s="118"/>
-      <c r="EV25" s="118"/>
-      <c r="EW25" s="118"/>
-      <c r="EX25" s="119"/>
+      <c r="EJ25" s="139"/>
+      <c r="EK25" s="139"/>
+      <c r="EL25" s="139"/>
+      <c r="EM25" s="139"/>
+      <c r="EN25" s="139"/>
+      <c r="EO25" s="139"/>
+      <c r="EP25" s="139"/>
+      <c r="EQ25" s="139"/>
+      <c r="ER25" s="139"/>
+      <c r="ES25" s="139"/>
+      <c r="ET25" s="139"/>
+      <c r="EU25" s="139"/>
+      <c r="EV25" s="139"/>
+      <c r="EW25" s="139"/>
+      <c r="EX25" s="140"/>
     </row>
     <row r="26" spans="1:154" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
@@ -3531,96 +3531,96 @@
       <c r="D26" s="66"/>
       <c r="E26" s="66"/>
       <c r="F26" s="66"/>
-      <c r="G26" s="156" t="s">
+      <c r="G26" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="156"/>
-      <c r="I26" s="156"/>
-      <c r="J26" s="156"/>
-      <c r="K26" s="157" t="s">
+      <c r="H26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="L26" s="157"/>
-      <c r="M26" s="157"/>
-      <c r="N26" s="157"/>
-      <c r="O26" s="157" t="s">
+      <c r="L26" s="119"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="P26" s="157"/>
-      <c r="Q26" s="157"/>
-      <c r="R26" s="157"/>
-      <c r="S26" s="142" t="s">
+      <c r="P26" s="119"/>
+      <c r="Q26" s="119"/>
+      <c r="R26" s="119"/>
+      <c r="S26" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="T26" s="142"/>
-      <c r="U26" s="142"/>
-      <c r="V26" s="142"/>
-      <c r="W26" s="142" t="s">
+      <c r="T26" s="120"/>
+      <c r="U26" s="120"/>
+      <c r="V26" s="120"/>
+      <c r="W26" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="X26" s="142"/>
-      <c r="Y26" s="142"/>
-      <c r="Z26" s="142"/>
-      <c r="AA26" s="142" t="s">
+      <c r="X26" s="120"/>
+      <c r="Y26" s="120"/>
+      <c r="Z26" s="120"/>
+      <c r="AA26" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="AB26" s="142"/>
-      <c r="AC26" s="142"/>
-      <c r="AD26" s="142"/>
-      <c r="AE26" s="142" t="s">
+      <c r="AB26" s="120"/>
+      <c r="AC26" s="120"/>
+      <c r="AD26" s="120"/>
+      <c r="AE26" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="AF26" s="142"/>
-      <c r="AG26" s="142"/>
-      <c r="AH26" s="142"/>
-      <c r="AI26" s="142" t="s">
+      <c r="AF26" s="120"/>
+      <c r="AG26" s="120"/>
+      <c r="AH26" s="120"/>
+      <c r="AI26" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="AJ26" s="142"/>
-      <c r="AK26" s="142"/>
-      <c r="AL26" s="142"/>
-      <c r="AM26" s="141" t="s">
+      <c r="AJ26" s="120"/>
+      <c r="AK26" s="120"/>
+      <c r="AL26" s="120"/>
+      <c r="AM26" s="131" t="s">
         <v>38</v>
       </c>
-      <c r="AN26" s="141"/>
-      <c r="AO26" s="141"/>
-      <c r="AP26" s="141"/>
-      <c r="AQ26" s="143" t="s">
+      <c r="AN26" s="131"/>
+      <c r="AO26" s="131"/>
+      <c r="AP26" s="131"/>
+      <c r="AQ26" s="132" t="s">
         <v>39</v>
       </c>
-      <c r="AR26" s="143"/>
-      <c r="AS26" s="143"/>
-      <c r="AT26" s="143"/>
-      <c r="AU26" s="144" t="s">
+      <c r="AR26" s="132"/>
+      <c r="AS26" s="132"/>
+      <c r="AT26" s="132"/>
+      <c r="AU26" s="136" t="s">
         <v>42</v>
       </c>
-      <c r="AV26" s="144"/>
-      <c r="AW26" s="144"/>
-      <c r="AX26" s="144"/>
-      <c r="AY26" s="142" t="s">
+      <c r="AV26" s="136"/>
+      <c r="AW26" s="136"/>
+      <c r="AX26" s="136"/>
+      <c r="AY26" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AZ26" s="142"/>
-      <c r="BA26" s="142"/>
-      <c r="BB26" s="142"/>
-      <c r="BC26" s="142" t="s">
+      <c r="AZ26" s="120"/>
+      <c r="BA26" s="120"/>
+      <c r="BB26" s="120"/>
+      <c r="BC26" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="BD26" s="142"/>
-      <c r="BE26" s="142"/>
-      <c r="BF26" s="142"/>
-      <c r="BG26" s="142" t="s">
+      <c r="BD26" s="120"/>
+      <c r="BE26" s="120"/>
+      <c r="BF26" s="120"/>
+      <c r="BG26" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="BH26" s="142"/>
-      <c r="BI26" s="142"/>
-      <c r="BJ26" s="142"/>
-      <c r="BK26" s="142" t="s">
+      <c r="BH26" s="120"/>
+      <c r="BI26" s="120"/>
+      <c r="BJ26" s="120"/>
+      <c r="BK26" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="BL26" s="142"/>
-      <c r="BM26" s="142"/>
-      <c r="BN26" s="142"/>
+      <c r="BL26" s="120"/>
+      <c r="BM26" s="120"/>
+      <c r="BN26" s="120"/>
       <c r="BQ26" s="78"/>
       <c r="BR26" s="79"/>
       <c r="BS26" s="80"/>
@@ -3628,108 +3628,108 @@
       <c r="BU26" s="80"/>
       <c r="BV26" s="14"/>
       <c r="BW26" s="14"/>
-      <c r="CI26" s="120" t="s">
+      <c r="CI26" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="CJ26" s="121"/>
-      <c r="CK26" s="121"/>
-      <c r="CL26" s="122"/>
-      <c r="CM26" s="120" t="s">
+      <c r="CJ26" s="134"/>
+      <c r="CK26" s="134"/>
+      <c r="CL26" s="135"/>
+      <c r="CM26" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="CN26" s="121"/>
-      <c r="CO26" s="121"/>
-      <c r="CP26" s="122"/>
-      <c r="CQ26" s="120" t="s">
+      <c r="CN26" s="134"/>
+      <c r="CO26" s="134"/>
+      <c r="CP26" s="135"/>
+      <c r="CQ26" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="CR26" s="121"/>
-      <c r="CS26" s="121"/>
-      <c r="CT26" s="122"/>
-      <c r="CU26" s="120" t="s">
+      <c r="CR26" s="134"/>
+      <c r="CS26" s="134"/>
+      <c r="CT26" s="135"/>
+      <c r="CU26" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="CV26" s="121"/>
-      <c r="CW26" s="121"/>
-      <c r="CX26" s="122"/>
-      <c r="CY26" s="120" t="s">
+      <c r="CV26" s="134"/>
+      <c r="CW26" s="134"/>
+      <c r="CX26" s="135"/>
+      <c r="CY26" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="CZ26" s="121"/>
-      <c r="DA26" s="121"/>
-      <c r="DB26" s="122"/>
-      <c r="DC26" s="141" t="s">
+      <c r="CZ26" s="134"/>
+      <c r="DA26" s="134"/>
+      <c r="DB26" s="135"/>
+      <c r="DC26" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="DD26" s="141"/>
-      <c r="DE26" s="141"/>
-      <c r="DF26" s="141"/>
-      <c r="DG26" s="120" t="s">
+      <c r="DD26" s="131"/>
+      <c r="DE26" s="131"/>
+      <c r="DF26" s="131"/>
+      <c r="DG26" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="DH26" s="121"/>
-      <c r="DI26" s="121"/>
-      <c r="DJ26" s="122"/>
-      <c r="DK26" s="120" t="s">
+      <c r="DH26" s="134"/>
+      <c r="DI26" s="134"/>
+      <c r="DJ26" s="135"/>
+      <c r="DK26" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="DL26" s="121"/>
-      <c r="DM26" s="121"/>
-      <c r="DN26" s="122"/>
-      <c r="DO26" s="120" t="s">
+      <c r="DL26" s="134"/>
+      <c r="DM26" s="134"/>
+      <c r="DN26" s="135"/>
+      <c r="DO26" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="DP26" s="121"/>
-      <c r="DQ26" s="121"/>
-      <c r="DR26" s="122"/>
-      <c r="DS26" s="120" t="s">
+      <c r="DP26" s="134"/>
+      <c r="DQ26" s="134"/>
+      <c r="DR26" s="135"/>
+      <c r="DS26" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="DT26" s="121"/>
-      <c r="DU26" s="121"/>
-      <c r="DV26" s="122"/>
-      <c r="DW26" s="120" t="s">
+      <c r="DT26" s="134"/>
+      <c r="DU26" s="134"/>
+      <c r="DV26" s="135"/>
+      <c r="DW26" s="133" t="s">
         <v>57</v>
       </c>
-      <c r="DX26" s="121"/>
-      <c r="DY26" s="121"/>
-      <c r="DZ26" s="122"/>
-      <c r="EA26" s="113" t="s">
+      <c r="DX26" s="134"/>
+      <c r="DY26" s="134"/>
+      <c r="DZ26" s="135"/>
+      <c r="EA26" s="158" t="s">
         <v>30</v>
       </c>
-      <c r="EB26" s="114"/>
-      <c r="EC26" s="114"/>
-      <c r="ED26" s="115"/>
-      <c r="EE26" s="110" t="s">
+      <c r="EB26" s="159"/>
+      <c r="EC26" s="159"/>
+      <c r="ED26" s="160"/>
+      <c r="EE26" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="EF26" s="111"/>
-      <c r="EG26" s="111"/>
-      <c r="EH26" s="112"/>
-      <c r="EI26" s="110" t="s">
+      <c r="EF26" s="156"/>
+      <c r="EG26" s="156"/>
+      <c r="EH26" s="157"/>
+      <c r="EI26" s="155" t="s">
         <v>58</v>
       </c>
-      <c r="EJ26" s="111"/>
-      <c r="EK26" s="111"/>
-      <c r="EL26" s="112"/>
-      <c r="EM26" s="120" t="s">
+      <c r="EJ26" s="156"/>
+      <c r="EK26" s="156"/>
+      <c r="EL26" s="157"/>
+      <c r="EM26" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="EN26" s="121"/>
-      <c r="EO26" s="121"/>
-      <c r="EP26" s="122"/>
-      <c r="EQ26" s="137" t="s">
+      <c r="EN26" s="134"/>
+      <c r="EO26" s="134"/>
+      <c r="EP26" s="135"/>
+      <c r="EQ26" s="152" t="s">
         <v>61</v>
       </c>
-      <c r="ER26" s="138"/>
-      <c r="ES26" s="138"/>
-      <c r="ET26" s="139"/>
-      <c r="EU26" s="120" t="s">
+      <c r="ER26" s="153"/>
+      <c r="ES26" s="153"/>
+      <c r="ET26" s="154"/>
+      <c r="EU26" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="EV26" s="121"/>
-      <c r="EW26" s="121"/>
-      <c r="EX26" s="122"/>
+      <c r="EV26" s="134"/>
+      <c r="EW26" s="134"/>
+      <c r="EX26" s="135"/>
     </row>
     <row r="27" spans="1:154" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
@@ -3738,96 +3738,96 @@
       <c r="D27" s="69"/>
       <c r="E27" s="69"/>
       <c r="F27" s="69"/>
-      <c r="G27" s="152">
+      <c r="G27" s="110">
         <v>1</v>
       </c>
-      <c r="H27" s="153"/>
-      <c r="I27" s="153"/>
-      <c r="J27" s="154"/>
-      <c r="K27" s="152">
+      <c r="H27" s="111"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="110">
         <v>2</v>
       </c>
-      <c r="L27" s="153"/>
-      <c r="M27" s="153"/>
-      <c r="N27" s="154"/>
-      <c r="O27" s="152">
+      <c r="L27" s="111"/>
+      <c r="M27" s="111"/>
+      <c r="N27" s="112"/>
+      <c r="O27" s="110">
         <v>3</v>
       </c>
-      <c r="P27" s="153"/>
-      <c r="Q27" s="153"/>
-      <c r="R27" s="154"/>
-      <c r="S27" s="152">
+      <c r="P27" s="111"/>
+      <c r="Q27" s="111"/>
+      <c r="R27" s="112"/>
+      <c r="S27" s="110">
         <v>4</v>
       </c>
-      <c r="T27" s="153"/>
-      <c r="U27" s="153"/>
-      <c r="V27" s="154"/>
-      <c r="W27" s="152">
+      <c r="T27" s="111"/>
+      <c r="U27" s="111"/>
+      <c r="V27" s="112"/>
+      <c r="W27" s="110">
         <v>5</v>
       </c>
-      <c r="X27" s="153"/>
-      <c r="Y27" s="153"/>
-      <c r="Z27" s="154"/>
-      <c r="AA27" s="152">
+      <c r="X27" s="111"/>
+      <c r="Y27" s="111"/>
+      <c r="Z27" s="112"/>
+      <c r="AA27" s="110">
         <v>6</v>
       </c>
-      <c r="AB27" s="153"/>
-      <c r="AC27" s="153"/>
-      <c r="AD27" s="154"/>
-      <c r="AE27" s="152">
+      <c r="AB27" s="111"/>
+      <c r="AC27" s="111"/>
+      <c r="AD27" s="112"/>
+      <c r="AE27" s="110">
         <v>7</v>
       </c>
-      <c r="AF27" s="153"/>
-      <c r="AG27" s="153"/>
-      <c r="AH27" s="154"/>
-      <c r="AI27" s="152">
+      <c r="AF27" s="111"/>
+      <c r="AG27" s="111"/>
+      <c r="AH27" s="112"/>
+      <c r="AI27" s="110">
         <v>8</v>
       </c>
-      <c r="AJ27" s="153"/>
-      <c r="AK27" s="153"/>
-      <c r="AL27" s="154"/>
-      <c r="AM27" s="152">
+      <c r="AJ27" s="111"/>
+      <c r="AK27" s="111"/>
+      <c r="AL27" s="112"/>
+      <c r="AM27" s="110">
         <v>9</v>
       </c>
-      <c r="AN27" s="153"/>
-      <c r="AO27" s="153"/>
-      <c r="AP27" s="154"/>
-      <c r="AQ27" s="152">
+      <c r="AN27" s="111"/>
+      <c r="AO27" s="111"/>
+      <c r="AP27" s="112"/>
+      <c r="AQ27" s="110">
         <v>10</v>
       </c>
-      <c r="AR27" s="153"/>
-      <c r="AS27" s="153"/>
-      <c r="AT27" s="154"/>
-      <c r="AU27" s="158">
+      <c r="AR27" s="111"/>
+      <c r="AS27" s="111"/>
+      <c r="AT27" s="112"/>
+      <c r="AU27" s="141">
         <v>11</v>
       </c>
-      <c r="AV27" s="159"/>
-      <c r="AW27" s="159"/>
-      <c r="AX27" s="160"/>
-      <c r="AY27" s="152">
+      <c r="AV27" s="142"/>
+      <c r="AW27" s="142"/>
+      <c r="AX27" s="143"/>
+      <c r="AY27" s="110">
         <v>12</v>
       </c>
-      <c r="AZ27" s="153"/>
-      <c r="BA27" s="153"/>
-      <c r="BB27" s="154"/>
-      <c r="BC27" s="152">
+      <c r="AZ27" s="111"/>
+      <c r="BA27" s="111"/>
+      <c r="BB27" s="112"/>
+      <c r="BC27" s="110">
         <v>13</v>
       </c>
-      <c r="BD27" s="153"/>
-      <c r="BE27" s="153"/>
-      <c r="BF27" s="154"/>
-      <c r="BG27" s="152">
+      <c r="BD27" s="111"/>
+      <c r="BE27" s="111"/>
+      <c r="BF27" s="112"/>
+      <c r="BG27" s="110">
         <v>14</v>
       </c>
-      <c r="BH27" s="153"/>
-      <c r="BI27" s="153"/>
-      <c r="BJ27" s="154"/>
-      <c r="BK27" s="152">
+      <c r="BH27" s="111"/>
+      <c r="BI27" s="111"/>
+      <c r="BJ27" s="112"/>
+      <c r="BK27" s="110">
         <v>15</v>
       </c>
-      <c r="BL27" s="153"/>
-      <c r="BM27" s="153"/>
-      <c r="BN27" s="154"/>
+      <c r="BL27" s="111"/>
+      <c r="BM27" s="111"/>
+      <c r="BN27" s="112"/>
       <c r="BQ27" s="81"/>
       <c r="BR27" s="82"/>
       <c r="BS27" s="78"/>
@@ -3835,108 +3835,108 @@
       <c r="BU27" s="78"/>
       <c r="BV27" s="14"/>
       <c r="BW27" s="14"/>
-      <c r="CI27" s="123">
+      <c r="CI27" s="124">
         <v>16</v>
       </c>
-      <c r="CJ27" s="124"/>
-      <c r="CK27" s="124"/>
-      <c r="CL27" s="125"/>
-      <c r="CM27" s="123">
+      <c r="CJ27" s="125"/>
+      <c r="CK27" s="125"/>
+      <c r="CL27" s="126"/>
+      <c r="CM27" s="124">
         <v>17</v>
       </c>
-      <c r="CN27" s="124"/>
-      <c r="CO27" s="124"/>
-      <c r="CP27" s="125"/>
-      <c r="CQ27" s="123">
+      <c r="CN27" s="125"/>
+      <c r="CO27" s="125"/>
+      <c r="CP27" s="126"/>
+      <c r="CQ27" s="124">
         <v>18</v>
       </c>
-      <c r="CR27" s="124"/>
-      <c r="CS27" s="124"/>
-      <c r="CT27" s="125"/>
-      <c r="CU27" s="123">
+      <c r="CR27" s="125"/>
+      <c r="CS27" s="125"/>
+      <c r="CT27" s="126"/>
+      <c r="CU27" s="124">
         <v>19</v>
       </c>
-      <c r="CV27" s="124"/>
-      <c r="CW27" s="124"/>
-      <c r="CX27" s="125"/>
-      <c r="CY27" s="123">
+      <c r="CV27" s="125"/>
+      <c r="CW27" s="125"/>
+      <c r="CX27" s="126"/>
+      <c r="CY27" s="124">
         <v>20</v>
       </c>
-      <c r="CZ27" s="124"/>
-      <c r="DA27" s="124"/>
-      <c r="DB27" s="125"/>
-      <c r="DC27" s="123">
+      <c r="CZ27" s="125"/>
+      <c r="DA27" s="125"/>
+      <c r="DB27" s="126"/>
+      <c r="DC27" s="124">
         <v>21</v>
       </c>
-      <c r="DD27" s="124"/>
-      <c r="DE27" s="124"/>
-      <c r="DF27" s="125"/>
-      <c r="DG27" s="123">
+      <c r="DD27" s="125"/>
+      <c r="DE27" s="125"/>
+      <c r="DF27" s="126"/>
+      <c r="DG27" s="124">
         <v>22</v>
       </c>
-      <c r="DH27" s="124"/>
-      <c r="DI27" s="124"/>
-      <c r="DJ27" s="125"/>
-      <c r="DK27" s="123">
+      <c r="DH27" s="125"/>
+      <c r="DI27" s="125"/>
+      <c r="DJ27" s="126"/>
+      <c r="DK27" s="124">
         <v>23</v>
       </c>
-      <c r="DL27" s="124"/>
-      <c r="DM27" s="124"/>
-      <c r="DN27" s="125"/>
-      <c r="DO27" s="123">
+      <c r="DL27" s="125"/>
+      <c r="DM27" s="125"/>
+      <c r="DN27" s="126"/>
+      <c r="DO27" s="124">
         <v>24</v>
       </c>
-      <c r="DP27" s="124"/>
-      <c r="DQ27" s="124"/>
-      <c r="DR27" s="125"/>
-      <c r="DS27" s="123">
+      <c r="DP27" s="125"/>
+      <c r="DQ27" s="125"/>
+      <c r="DR27" s="126"/>
+      <c r="DS27" s="124">
         <v>25</v>
       </c>
-      <c r="DT27" s="124"/>
-      <c r="DU27" s="124"/>
-      <c r="DV27" s="125"/>
-      <c r="DW27" s="123">
+      <c r="DT27" s="125"/>
+      <c r="DU27" s="125"/>
+      <c r="DV27" s="126"/>
+      <c r="DW27" s="124">
         <v>26</v>
       </c>
-      <c r="DX27" s="124"/>
-      <c r="DY27" s="124"/>
-      <c r="DZ27" s="125"/>
-      <c r="EA27" s="123">
+      <c r="DX27" s="125"/>
+      <c r="DY27" s="125"/>
+      <c r="DZ27" s="126"/>
+      <c r="EA27" s="124">
         <v>27</v>
       </c>
-      <c r="EB27" s="124"/>
-      <c r="EC27" s="124"/>
-      <c r="ED27" s="125"/>
-      <c r="EE27" s="123">
+      <c r="EB27" s="125"/>
+      <c r="EC27" s="125"/>
+      <c r="ED27" s="126"/>
+      <c r="EE27" s="124">
         <v>28</v>
       </c>
-      <c r="EF27" s="124"/>
-      <c r="EG27" s="124"/>
-      <c r="EH27" s="125"/>
-      <c r="EI27" s="123">
+      <c r="EF27" s="125"/>
+      <c r="EG27" s="125"/>
+      <c r="EH27" s="126"/>
+      <c r="EI27" s="124">
         <v>29</v>
       </c>
-      <c r="EJ27" s="124"/>
-      <c r="EK27" s="124"/>
-      <c r="EL27" s="125"/>
-      <c r="EM27" s="123">
+      <c r="EJ27" s="125"/>
+      <c r="EK27" s="125"/>
+      <c r="EL27" s="126"/>
+      <c r="EM27" s="124">
         <v>30</v>
       </c>
-      <c r="EN27" s="124"/>
-      <c r="EO27" s="124"/>
-      <c r="EP27" s="125"/>
-      <c r="EQ27" s="123">
+      <c r="EN27" s="125"/>
+      <c r="EO27" s="125"/>
+      <c r="EP27" s="126"/>
+      <c r="EQ27" s="124">
         <v>31</v>
       </c>
-      <c r="ER27" s="124"/>
-      <c r="ES27" s="124"/>
-      <c r="ET27" s="125"/>
-      <c r="EU27" s="123">
+      <c r="ER27" s="125"/>
+      <c r="ES27" s="125"/>
+      <c r="ET27" s="126"/>
+      <c r="EU27" s="124">
         <v>32</v>
       </c>
-      <c r="EV27" s="124"/>
-      <c r="EW27" s="124"/>
-      <c r="EX27" s="125"/>
+      <c r="EV27" s="125"/>
+      <c r="EW27" s="125"/>
+      <c r="EX27" s="126"/>
     </row>
     <row r="28" spans="1:154" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
@@ -5992,82 +5992,18 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="W27:Z27"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="H13:S13"/>
-    <mergeCell ref="H14:S14"/>
-    <mergeCell ref="H17:S17"/>
-    <mergeCell ref="U12:Z12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H15:S15"/>
-    <mergeCell ref="H16:S16"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="O26:R26"/>
-    <mergeCell ref="S26:V26"/>
-    <mergeCell ref="W26:Z26"/>
-    <mergeCell ref="P25:AF25"/>
-    <mergeCell ref="AA27:AD27"/>
-    <mergeCell ref="AE27:AH27"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="U13:Z13"/>
-    <mergeCell ref="U14:Z14"/>
-    <mergeCell ref="U17:Z17"/>
-    <mergeCell ref="CI27:CL27"/>
-    <mergeCell ref="CM27:CP27"/>
-    <mergeCell ref="CQ27:CT27"/>
-    <mergeCell ref="CU27:CX27"/>
-    <mergeCell ref="G25:O25"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="AB17:AM17"/>
-    <mergeCell ref="AO17:AT17"/>
-    <mergeCell ref="AQ15:AR15"/>
-    <mergeCell ref="AO12:AT12"/>
-    <mergeCell ref="AB13:AM13"/>
-    <mergeCell ref="AB14:AM14"/>
-    <mergeCell ref="AQ14:AR14"/>
-    <mergeCell ref="AQ13:AR13"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="AA26:AD26"/>
-    <mergeCell ref="AE26:AH26"/>
-    <mergeCell ref="AI26:AL26"/>
-    <mergeCell ref="AM26:AP26"/>
-    <mergeCell ref="AQ26:AT26"/>
-    <mergeCell ref="CY26:DB26"/>
-    <mergeCell ref="AU26:AX26"/>
-    <mergeCell ref="AY26:BB26"/>
-    <mergeCell ref="BC26:BF26"/>
-    <mergeCell ref="BG26:BJ26"/>
-    <mergeCell ref="BK26:BN26"/>
-    <mergeCell ref="AG25:AW25"/>
-    <mergeCell ref="AX25:BO25"/>
-    <mergeCell ref="CJ25:CY25"/>
-    <mergeCell ref="CZ25:DR25"/>
-    <mergeCell ref="DO27:DR27"/>
-    <mergeCell ref="DS27:DV27"/>
-    <mergeCell ref="DW27:DZ27"/>
-    <mergeCell ref="DC26:DF26"/>
-    <mergeCell ref="DG26:DJ26"/>
-    <mergeCell ref="DK26:DN26"/>
-    <mergeCell ref="DO26:DR26"/>
-    <mergeCell ref="CY27:DB27"/>
-    <mergeCell ref="DC27:DF27"/>
-    <mergeCell ref="DG27:DJ27"/>
-    <mergeCell ref="DK27:DN27"/>
-    <mergeCell ref="AU27:AX27"/>
-    <mergeCell ref="AY27:BB27"/>
-    <mergeCell ref="BC27:BF27"/>
-    <mergeCell ref="BG27:BJ27"/>
-    <mergeCell ref="BK27:BN27"/>
-    <mergeCell ref="AI27:AL27"/>
-    <mergeCell ref="AM27:AP27"/>
-    <mergeCell ref="AQ27:AT27"/>
+    <mergeCell ref="EI26:EL26"/>
+    <mergeCell ref="EE26:EH26"/>
+    <mergeCell ref="EA26:ED26"/>
+    <mergeCell ref="BH17:BN17"/>
+    <mergeCell ref="DS25:EH25"/>
+    <mergeCell ref="EI25:EX25"/>
+    <mergeCell ref="DS26:DV26"/>
+    <mergeCell ref="DW26:DZ26"/>
+    <mergeCell ref="CI26:CL26"/>
+    <mergeCell ref="CM26:CP26"/>
+    <mergeCell ref="CQ26:CT26"/>
+    <mergeCell ref="CU26:CX26"/>
     <mergeCell ref="EU27:EX27"/>
     <mergeCell ref="EA27:ED27"/>
     <mergeCell ref="EE27:EH27"/>
@@ -6092,18 +6028,82 @@
     <mergeCell ref="EU26:EX26"/>
     <mergeCell ref="EQ26:ET26"/>
     <mergeCell ref="EM26:EP26"/>
-    <mergeCell ref="EI26:EL26"/>
-    <mergeCell ref="EE26:EH26"/>
-    <mergeCell ref="EA26:ED26"/>
-    <mergeCell ref="BH17:BN17"/>
-    <mergeCell ref="DS25:EH25"/>
-    <mergeCell ref="EI25:EX25"/>
-    <mergeCell ref="DS26:DV26"/>
-    <mergeCell ref="DW26:DZ26"/>
-    <mergeCell ref="CI26:CL26"/>
-    <mergeCell ref="CM26:CP26"/>
-    <mergeCell ref="CQ26:CT26"/>
-    <mergeCell ref="CU26:CX26"/>
+    <mergeCell ref="DO27:DR27"/>
+    <mergeCell ref="DS27:DV27"/>
+    <mergeCell ref="DW27:DZ27"/>
+    <mergeCell ref="DC26:DF26"/>
+    <mergeCell ref="DG26:DJ26"/>
+    <mergeCell ref="DK26:DN26"/>
+    <mergeCell ref="DO26:DR26"/>
+    <mergeCell ref="CY27:DB27"/>
+    <mergeCell ref="DC27:DF27"/>
+    <mergeCell ref="DG27:DJ27"/>
+    <mergeCell ref="DK27:DN27"/>
+    <mergeCell ref="CY26:DB26"/>
+    <mergeCell ref="AU26:AX26"/>
+    <mergeCell ref="AY26:BB26"/>
+    <mergeCell ref="BC26:BF26"/>
+    <mergeCell ref="BG26:BJ26"/>
+    <mergeCell ref="BK26:BN26"/>
+    <mergeCell ref="AG25:AW25"/>
+    <mergeCell ref="AX25:BO25"/>
+    <mergeCell ref="CJ25:CY25"/>
+    <mergeCell ref="CZ25:DR25"/>
+    <mergeCell ref="AQ15:AR15"/>
+    <mergeCell ref="AO12:AT12"/>
+    <mergeCell ref="AB13:AM13"/>
+    <mergeCell ref="AB14:AM14"/>
+    <mergeCell ref="AQ14:AR14"/>
+    <mergeCell ref="AQ13:AR13"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="AA26:AD26"/>
+    <mergeCell ref="AE26:AH26"/>
+    <mergeCell ref="AI26:AL26"/>
+    <mergeCell ref="AM26:AP26"/>
+    <mergeCell ref="AQ26:AT26"/>
+    <mergeCell ref="AI27:AL27"/>
+    <mergeCell ref="AM27:AP27"/>
+    <mergeCell ref="AQ27:AT27"/>
+    <mergeCell ref="CI27:CL27"/>
+    <mergeCell ref="CM27:CP27"/>
+    <mergeCell ref="CQ27:CT27"/>
+    <mergeCell ref="CU27:CX27"/>
+    <mergeCell ref="G25:O25"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="AB17:AM17"/>
+    <mergeCell ref="AO17:AT17"/>
+    <mergeCell ref="AU27:AX27"/>
+    <mergeCell ref="AY27:BB27"/>
+    <mergeCell ref="BC27:BF27"/>
+    <mergeCell ref="BG27:BJ27"/>
+    <mergeCell ref="BK27:BN27"/>
+    <mergeCell ref="W27:Z27"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="H13:S13"/>
+    <mergeCell ref="H14:S14"/>
+    <mergeCell ref="H17:S17"/>
+    <mergeCell ref="U12:Z12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H15:S15"/>
+    <mergeCell ref="H16:S16"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="W26:Z26"/>
+    <mergeCell ref="P25:AF25"/>
+    <mergeCell ref="AA27:AD27"/>
+    <mergeCell ref="AE27:AH27"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="U13:Z13"/>
+    <mergeCell ref="U14:Z14"/>
+    <mergeCell ref="U17:Z17"/>
   </mergeCells>
   <conditionalFormatting sqref="G25">
     <cfRule type="expression" dxfId="6" priority="19">

</xml_diff>